<commit_message>
Fix wording of indicators survey
</commit_message>
<xml_diff>
--- a/app/config/tables/indicators/forms/indicators/indicators.xlsx
+++ b/app/config/tables/indicators/forms/indicators/indicators.xlsx
@@ -438,19 +438,19 @@
     <t>data('voltage_stabilizer_working') === 0</t>
   </si>
   <si>
-    <t>How many heat alarms with over 10 hour duration above 8°C show in the termperature log from the 1st of the month to the last day of the month?</t>
-  </si>
-  <si>
-    <t>How many freeze alarms with over 1 hour duration below -0.5°C show in the temperature log for the 1st of the month to the last day of the month?</t>
-  </si>
-  <si>
-    <t>How many heat alarms with 48 hour or longer duration in the temperature log for the 1st of the month to the last day of the month?</t>
-  </si>
-  <si>
-    <t>Have there been any issues related to build quality from the 1st of the month to the last day of the month?</t>
-  </si>
-  <si>
-    <t>Has the voltage regulator been replaced from the 1st of the month to the last day of the month?</t>
+    <t>How many heat alarms with over 10 hour duration above 8°C show in the termperature log from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>How many freeze alarms with over 1 hour duration below -0.5°C show in the temperature log from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>How many heat alarms with 48 hour or longer duration in the temperature log from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>Have there been any issues related to build quality from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>Has the voltage regulator been replaced from the first day of the month to the last day of the month?</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify indicators based on PATH suggestions
</commit_message>
<xml_diff>
--- a/app/config/tables/indicators/forms/indicators/indicators.xlsx
+++ b/app/config/tables/indicators/forms/indicators/indicators.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11055" yWindow="0" windowWidth="3390" windowHeight="1350" tabRatio="500"/>
+    <workbookView xWindow="11052" yWindow="0" windowWidth="3396" windowHeight="1356" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="queries" sheetId="3" r:id="rId3"/>
-    <sheet name="settings" sheetId="4" r:id="rId4"/>
-    <sheet name="properties" sheetId="5" r:id="rId5"/>
+    <sheet name="calculates" sheetId="7" r:id="rId2"/>
+    <sheet name="model" sheetId="6" r:id="rId3"/>
+    <sheet name="choices" sheetId="2" r:id="rId4"/>
+    <sheet name="queries" sheetId="3" r:id="rId5"/>
+    <sheet name="settings" sheetId="4" r:id="rId6"/>
+    <sheet name="properties" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="177">
   <si>
     <t>clause</t>
   </si>
@@ -81,24 +83,9 @@
     <t>Por favor entre el ID del frigorífico</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>date_serviced</t>
   </si>
   <si>
-    <t>Date Serviced</t>
-  </si>
-  <si>
-    <t>Fecha de Servicio</t>
-  </si>
-  <si>
-    <t>Enter the date of service</t>
-  </si>
-  <si>
-    <t>Fecha de servicio</t>
-  </si>
-  <si>
     <t>choice_list_name</t>
   </si>
   <si>
@@ -270,9 +257,6 @@
     <t>config/tables/indicators/html/indicators_list.html</t>
   </si>
   <si>
-    <t>select_one_integer</t>
-  </si>
-  <si>
     <t>functional</t>
   </si>
   <si>
@@ -291,15 +275,6 @@
     <t>functional_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Is the refrigerator working properly? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 or more heat alarms in a month = Non-functional 
-1 or more freeze alarms in a month = Non-functional
-1 or more heat alarms with duration of 48 hrs or more = Non-functional
- </t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -423,21 +398,6 @@
     <t>display.hint.text.es</t>
   </si>
   <si>
-    <t>selected(data('build_quality'), 1)</t>
-  </si>
-  <si>
-    <t>selected(data('voltage_stabilizer_replaced'), 1)</t>
-  </si>
-  <si>
-    <t>selected(data('warranty_claim_been_made'), 1)</t>
-  </si>
-  <si>
-    <t>data('functional') === 0</t>
-  </si>
-  <si>
-    <t>data('voltage_stabilizer_working') === 0</t>
-  </si>
-  <si>
     <t>How many heat alarms with over 10 hour duration above 8°C show in the termperature log from the first day of the month to the last day of the month?</t>
   </si>
   <si>
@@ -451,13 +411,171 @@
   </si>
   <si>
     <t>Has the voltage regulator been replaced from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>non_functional</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>alarm_functional_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t>voltage_stabilizer_present</t>
+  </si>
+  <si>
+    <t>isSessionVariable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t>data('voltage_stabilizer_present') !== 'no'</t>
+  </si>
+  <si>
+    <t>yes_no_na</t>
+  </si>
+  <si>
+    <t>n_a</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>selected(data('build_quality'), 'yes')</t>
+  </si>
+  <si>
+    <t>data('voltage_stabilizer_working') === 'no'</t>
+  </si>
+  <si>
+    <t>selected(data('voltage_stabilizer_replaced'), 'yes')</t>
+  </si>
+  <si>
+    <t>selected(data('warranty_claim_been_made'), 'yes')</t>
+  </si>
+  <si>
+    <t>data('refrigerator_id') === null || data('refrigerator_id') === undefined</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Refrigerator ID: {{data.refrigerator_id}}</t>
+  </si>
+  <si>
+    <t>ID de Frigorífico: {{data.refrigerator_id}}</t>
+  </si>
+  <si>
+    <t>calculation_name</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>non_functional_calc</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>calculates.non_functional_calc()</t>
+  </si>
+  <si>
+    <t>data('alarm_functional_status') === 'non_functional'</t>
+  </si>
+  <si>
+    <t>reporting_period</t>
+  </si>
+  <si>
+    <t>Período de información</t>
+  </si>
+  <si>
+    <t>Reporting Period</t>
+  </si>
+  <si>
+    <t>Enter the date for the reporting period</t>
+  </si>
+  <si>
+    <t>refrigerator_age</t>
+  </si>
+  <si>
+    <t>year_installed</t>
+  </si>
+  <si>
+    <t>(function() {
+var frigYear = data('year_installed');
+if (data('year_installed') === null || data('year_installed') === undefined || data('year_installed') === 0) { return 0; }
+var currYear = new Date().getFullYear();
+var years = Math.abs(currYear - frigYear);
+return years;})()</t>
+  </si>
+  <si>
+    <t>calculates.refrigerator_age() &lt; 4</t>
+  </si>
+  <si>
+    <t>second_build_quality_issue</t>
+  </si>
+  <si>
+    <t>third_build_quality_issue</t>
+  </si>
+  <si>
+    <t>build_quality2</t>
+  </si>
+  <si>
+    <t>selected(data('build_quality2'), 'yes')</t>
+  </si>
+  <si>
+    <t>build_quality_reason2</t>
+  </si>
+  <si>
+    <t>build_quality_image2</t>
+  </si>
+  <si>
+    <t>build_quality3</t>
+  </si>
+  <si>
+    <t>Was there a second issue related to build quality from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>Was there a third issue related to build quality from the first day of the month to the last day of the month?</t>
+  </si>
+  <si>
+    <t>build_quality_reason3</t>
+  </si>
+  <si>
+    <t>build_quality_image3</t>
+  </si>
+  <si>
+    <t>selected(data('build_quality3'), 'yes')</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if </t>
+  </si>
+  <si>
+    <t>((data('heat_alarms') &gt;=  5 || data('freeze_alarms') &gt;=  1 || data('heat_alarms_over_48') &gt;=  1) ? 'non_functional' : 'functional')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -501,6 +619,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -568,7 +691,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -594,6 +717,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1040,27 +1164,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
-    <col min="5" max="5" width="37.125" customWidth="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1"/>
-    <col min="7" max="7" width="32.375" customWidth="1"/>
-    <col min="8" max="8" width="24.625" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="2" max="2" width="37.19921875" customWidth="1"/>
+    <col min="3" max="3" width="32.8984375" customWidth="1"/>
+    <col min="4" max="4" width="22.59765625" customWidth="1"/>
+    <col min="5" max="5" width="37.09765625" customWidth="1"/>
+    <col min="6" max="6" width="32.8984375" customWidth="1"/>
+    <col min="7" max="7" width="32.3984375" customWidth="1"/>
+    <col min="8" max="8" width="24.59765625" customWidth="1"/>
     <col min="9" max="9" width="39.5" customWidth="1"/>
-    <col min="10" max="1025" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="24.69921875" customWidth="1"/>
+    <col min="12" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,18 +1209,21 @@
         <v>8</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1105,364 +1234,637 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="b">
+      <c r="J4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="126" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="F6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
         <v>85</v>
       </c>
-      <c r="E6" t="s">
+      <c r="J17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" t="s">
+        <v>171</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" t="s">
+        <v>107</v>
+      </c>
+      <c r="F59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E61" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D67" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" t="s">
+        <v>111</v>
+      </c>
+      <c r="F67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>174</v>
+      </c>
+      <c r="E69" t="s">
+        <v>113</v>
+      </c>
+      <c r="F69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
         <v>80</v>
       </c>
-      <c r="F6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="E70" t="s">
         <v>115</v>
       </c>
-      <c r="F27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="F70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>118</v>
       </c>
-      <c r="E29" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" t="s">
-        <v>119</v>
-      </c>
-      <c r="F33" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" t="s">
-        <v>121</v>
-      </c>
-      <c r="F35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
-      <c r="E36" t="s">
-        <v>123</v>
-      </c>
-      <c r="F36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>126</v>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1478,27 +1880,155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" customWidth="1"/>
+    <col min="2" max="2" width="71.09765625" customWidth="1"/>
+    <col min="7" max="7" width="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.09765625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
     <col min="5" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1507,98 +2037,140 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
       </c>
       <c r="C6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +2184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1620,69 +2192,69 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="29.8984375" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="47.125" customWidth="1"/>
-    <col min="8" max="8" width="38.875" customWidth="1"/>
+    <col min="7" max="7" width="47.09765625" customWidth="1"/>
+    <col min="8" max="8" width="38.8984375" customWidth="1"/>
     <col min="9" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +2268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1704,22 +2276,22 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" customWidth="1"/>
+    <col min="4" max="4" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="29.09765625" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1728,75 +2300,75 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>20190826</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F8" t="s">
         <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1810,7 +2382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1818,149 +2390,149 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added observation, location, and component to the build quality questions
</commit_message>
<xml_diff>
--- a/app/config/tables/indicators/forms/indicators/indicators.xlsx
+++ b/app/config/tables/indicators/forms/indicators/indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11055" yWindow="0" windowWidth="3390" windowHeight="1350" tabRatio="500"/>
+    <workbookView xWindow="11060" yWindow="0" windowWidth="3390" windowHeight="1350" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,11 @@
     <sheet name="properties" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="240">
   <si>
     <t>clause</t>
   </si>
@@ -569,6 +561,195 @@
 var currYear = new Date().getFullYear();
 var years = Math.abs(currYear - frigYear);
 return years;})()</t>
+  </si>
+  <si>
+    <t>Refrigerator Status: {{data.alarm_functional_status}}</t>
+  </si>
+  <si>
+    <t>Estado del refrigerador: {{data.alarm_functional_status}}</t>
+  </si>
+  <si>
+    <t>build_quality_observation</t>
+  </si>
+  <si>
+    <t>build_quality_location</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>build_quality_component</t>
+  </si>
+  <si>
+    <t>build_quality_observation2</t>
+  </si>
+  <si>
+    <t>build_quality_location2</t>
+  </si>
+  <si>
+    <t>build_quality_component2</t>
+  </si>
+  <si>
+    <t>build_quality_observation3</t>
+  </si>
+  <si>
+    <t>build_quality_location3</t>
+  </si>
+  <si>
+    <t>build_quality_component3</t>
+  </si>
+  <si>
+    <t>build_quality_reason_type_observation</t>
+  </si>
+  <si>
+    <t>build_quality_reason_type_location</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>burnt</t>
+  </si>
+  <si>
+    <t>corrosion</t>
+  </si>
+  <si>
+    <t>deteriorating</t>
+  </si>
+  <si>
+    <t>leaking</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>noisy</t>
+  </si>
+  <si>
+    <t>Burnt</t>
+  </si>
+  <si>
+    <t>Corrosion</t>
+  </si>
+  <si>
+    <t>Deteriorating</t>
+  </si>
+  <si>
+    <t>Leaking</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Noisy</t>
+  </si>
+  <si>
+    <t>Broken</t>
+  </si>
+  <si>
+    <t>appliance_exterior</t>
+  </si>
+  <si>
+    <t>accessory_ems</t>
+  </si>
+  <si>
+    <t>solar_mechanical</t>
+  </si>
+  <si>
+    <t>solar_electrical</t>
+  </si>
+  <si>
+    <t>appliance_interior</t>
+  </si>
+  <si>
+    <t>not_determined</t>
+  </si>
+  <si>
+    <t>Accessory (EMS)</t>
+  </si>
+  <si>
+    <t>Solar (mechanical)</t>
+  </si>
+  <si>
+    <t>Solar (electrical)</t>
+  </si>
+  <si>
+    <t>Appliance (interior)</t>
+  </si>
+  <si>
+    <t>Not Determined</t>
+  </si>
+  <si>
+    <t>Appliance (exterior)</t>
+  </si>
+  <si>
+    <t>Roto</t>
+  </si>
+  <si>
+    <t>Quemado</t>
+  </si>
+  <si>
+    <t>Corrosión</t>
+  </si>
+  <si>
+    <t>Deterioro</t>
+  </si>
+  <si>
+    <t>Fugas</t>
+  </si>
+  <si>
+    <t>Desaparecido</t>
+  </si>
+  <si>
+    <t>Ruidoso</t>
+  </si>
+  <si>
+    <t>Aparato (exterior)</t>
+  </si>
+  <si>
+    <t>Aparato (interior)</t>
+  </si>
+  <si>
+    <t>Accesorio (EMS)</t>
+  </si>
+  <si>
+    <t>Solar (mecánica)</t>
+  </si>
+  <si>
+    <t>Solar (eléctrico)</t>
+  </si>
+  <si>
+    <t>No determinado</t>
+  </si>
+  <si>
+    <t>Necesita datos</t>
+  </si>
+  <si>
+    <t>Please enter the component that failed, and why if known.</t>
+  </si>
+  <si>
+    <t>Where was the failure observed?</t>
+  </si>
+  <si>
+    <t>What condition was observed related to the failure?</t>
+  </si>
+  <si>
+    <t>What condition was observed related to the second failure?</t>
+  </si>
+  <si>
+    <t>Where was the second failure observed?</t>
+  </si>
+  <si>
+    <t>Please enter the second component that failed, and why if known.</t>
+  </si>
+  <si>
+    <t>What condition was observed related to the third failure?</t>
+  </si>
+  <si>
+    <t>Where was the third failure observed?</t>
+  </si>
+  <si>
+    <t>Please enter the third component that failed, and why if known.</t>
   </si>
 </sst>
 </file>
@@ -691,7 +872,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -718,6 +899,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1164,29 +1347,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="37.25" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
-    <col min="5" max="5" width="37.125" customWidth="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1"/>
-    <col min="7" max="7" width="32.375" customWidth="1"/>
-    <col min="8" max="8" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="34.25" customWidth="1"/>
+    <col min="5" max="5" width="37.08203125" customWidth="1"/>
+    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.58203125" customWidth="1"/>
     <col min="9" max="9" width="39.5" customWidth="1"/>
     <col min="10" max="10" width="8.5" customWidth="1"/>
     <col min="11" max="11" width="24.75" customWidth="1"/>
     <col min="12" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1404,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
@@ -1234,7 +1417,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
@@ -1249,7 +1432,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1275,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -1283,7 +1466,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -1297,7 +1480,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>173</v>
       </c>
@@ -1321,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -1332,7 +1515,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>80</v>
       </c>
@@ -1346,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>80</v>
       </c>
@@ -1360,12 +1543,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>80</v>
       </c>
@@ -1379,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>151</v>
       </c>
@@ -1390,17 +1573,17 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1408,407 +1591,446 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" t="s">
+        <v>177</v>
+      </c>
+      <c r="G17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>86</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>89</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>85</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
         <v>129</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>91</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>90</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>94</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
         <v>84</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>101</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>99</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" t="s">
+        <v>182</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
         <v>129</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D35" t="s">
         <v>91</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E35" t="s">
         <v>163</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F35" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>94</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B36" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
         <v>84</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D37" t="s">
         <v>101</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E37" t="s">
         <v>165</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F37" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" t="s">
+        <v>183</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>94</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B44" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
         <v>96</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E46" t="s">
         <v>166</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F46" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
         <v>129</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D51" t="s">
         <v>91</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E51" t="s">
         <v>167</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F51" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>94</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B52" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
         <v>84</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D53" t="s">
         <v>101</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E53" t="s">
         <v>170</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F53" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E55" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>181</v>
+      </c>
+      <c r="E56" t="s">
+        <v>188</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
-      <c r="E48" t="s">
-        <v>171</v>
-      </c>
-      <c r="F48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>134</v>
-      </c>
-      <c r="B51" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>129</v>
-      </c>
-      <c r="D53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" t="s">
-        <v>102</v>
-      </c>
-      <c r="F53" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" t="s">
-        <v>106</v>
-      </c>
-      <c r="E55" t="s">
-        <v>104</v>
-      </c>
-      <c r="F55" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" t="s">
-        <v>91</v>
-      </c>
-      <c r="E59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F59" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>94</v>
       </c>
       <c r="B60" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>84</v>
-      </c>
-      <c r="D61" t="s">
-        <v>110</v>
-      </c>
-      <c r="E61" t="s">
-        <v>108</v>
-      </c>
-      <c r="F61" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>96</v>
+      </c>
+      <c r="E62" t="s">
+        <v>171</v>
+      </c>
+      <c r="F62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C67" t="s">
         <v>129</v>
       </c>
@@ -1816,65 +2038,175 @@
         <v>91</v>
       </c>
       <c r="E67" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>94</v>
       </c>
       <c r="B68" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" t="s">
+        <v>104</v>
+      </c>
+      <c r="F69" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C73" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E75" t="s">
+        <v>108</v>
+      </c>
+      <c r="F75" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C81" t="s">
+        <v>129</v>
+      </c>
+      <c r="D81" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" t="s">
+        <v>111</v>
+      </c>
+      <c r="F81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
         <v>173</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E83" t="s">
         <v>113</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F83" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
         <v>80</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E84" t="s">
         <v>115</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F84" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1886,14 +2218,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.75" customWidth="1"/>
-    <col min="2" max="2" width="71.125" customWidth="1"/>
+    <col min="2" max="2" width="71.08203125" customWidth="1"/>
     <col min="7" max="7" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>148</v>
       </c>
@@ -1901,7 +2233,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>150</v>
       </c>
@@ -1910,7 +2242,7 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -1931,12 +2263,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.625" customWidth="1"/>
+    <col min="2" max="2" width="28.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1947,7 +2279,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1955,7 +2287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -1963,7 +2295,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1971,7 +2303,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1979,7 +2311,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1990,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -2008,22 +2340,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A30" sqref="A30:A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -2037,7 +2369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2051,7 +2383,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -2065,7 +2397,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -2075,8 +2407,11 @@
       <c r="C5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2086,8 +2421,11 @@
       <c r="C6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2097,8 +2435,11 @@
       <c r="C8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>101</v>
       </c>
@@ -2108,8 +2449,11 @@
       <c r="C10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -2119,8 +2463,11 @@
       <c r="C12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -2130,8 +2477,11 @@
       <c r="C14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -2145,7 +2495,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -2159,7 +2509,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -2171,16 +2521,195 @@
       </c>
       <c r="D18" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2192,20 +2721,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="47.125" customWidth="1"/>
-    <col min="8" max="8" width="38.875" customWidth="1"/>
+    <col min="7" max="7" width="47.08203125" customWidth="1"/>
+    <col min="8" max="8" width="38.83203125" customWidth="1"/>
     <col min="9" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2231,7 +2760,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2276,17 +2805,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.08203125" customWidth="1"/>
+    <col min="5" max="5" width="29.08203125" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2306,7 +2835,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2314,7 +2843,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2322,7 +2851,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -2333,7 +2862,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>40</v>
       </c>
@@ -2341,7 +2870,7 @@
         <v>20190826</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2349,7 +2878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2360,7 +2889,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2390,16 +2919,16 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="22.58203125" customWidth="1"/>
+    <col min="4" max="4" width="20.08203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -2416,7 +2945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>51</v>
       </c>
@@ -2433,7 +2962,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -2450,7 +2979,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>51</v>
       </c>
@@ -2467,7 +2996,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -2484,7 +3013,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -2501,7 +3030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -2518,7 +3047,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Address warranty claim in indicators
</commit_message>
<xml_diff>
--- a/app/config/tables/indicators/forms/indicators/indicators.xlsx
+++ b/app/config/tables/indicators/forms/indicators/indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="0" windowWidth="3390" windowHeight="1350" tabRatio="500"/>
+    <workbookView xWindow="11055" yWindow="0" windowWidth="3390" windowHeight="1350" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="8" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="settings" sheetId="4" r:id="rId7"/>
     <sheet name="properties" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="302">
   <si>
     <t>clause</t>
   </si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>year_installed</t>
-  </si>
-  <si>
-    <t>calculates.refrigerator_age() &lt; 4</t>
   </si>
   <si>
     <t>second_build_quality_issue</t>
@@ -936,6 +933,12 @@
   </si>
   <si>
     <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
+    <t>power_source</t>
+  </si>
+  <si>
+    <t>(calculates.refrigerator_age() &lt; 4 || (calculates.refrigerator_age() &lt; 11 &amp;&amp; data('power_source') === 'solar'))</t>
   </si>
 </sst>
 </file>
@@ -1555,11 +1558,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="23" customWidth="1"/>
     <col min="2" max="2" width="8.75" style="23"/>
@@ -1568,7 +1571,7 @@
     <col min="5" max="16384" width="8.75" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1576,27 +1579,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="21" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>298</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
     </row>
-    <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -1610,20 +1613,20 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="37.25" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.875" customWidth="1"/>
     <col min="4" max="4" width="34.25" customWidth="1"/>
-    <col min="5" max="5" width="37.08203125" customWidth="1"/>
+    <col min="5" max="5" width="37.125" customWidth="1"/>
     <col min="6" max="6" width="51" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="43.83203125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="24.58203125" customWidth="1"/>
+    <col min="8" max="8" width="43.875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="24.625" customWidth="1"/>
     <col min="10" max="10" width="39.5" customWidth="1"/>
     <col min="11" max="11" width="39.5" style="12" customWidth="1"/>
     <col min="12" max="12" width="8.5" customWidth="1"/>
@@ -1631,7 +1634,7 @@
     <col min="14" max="1027" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>116</v>
@@ -1663,7 +1666,7 @@
         <v>117</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1672,7 +1675,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>114</v>
       </c>
@@ -1687,7 +1690,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
@@ -1704,7 +1707,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1721,7 +1724,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -1733,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -1741,7 +1744,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -1755,12 +1758,12 @@
         <v>144</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
@@ -1773,7 +1776,7 @@
         <v>152</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>154</v>
@@ -1786,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1798,7 +1801,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>80</v>
       </c>
@@ -1809,13 +1812,13 @@
         <v>118</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>80</v>
       </c>
@@ -1826,18 +1829,18 @@
         <v>119</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>80</v>
       </c>
@@ -1848,13 +1851,13 @@
         <v>120</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>148</v>
       </c>
@@ -1865,17 +1868,17 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1883,23 +1886,23 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>142</v>
       </c>
       <c r="F17" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" t="s">
         <v>172</v>
       </c>
-      <c r="G17" t="s">
-        <v>173</v>
-      </c>
       <c r="H17" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
         <v>89</v>
@@ -1908,18 +1911,18 @@
         <v>85</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>126</v>
       </c>
@@ -1933,10 +1936,10 @@
         <v>121</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1944,65 +1947,65 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>126</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>175</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>176</v>
       </c>
-      <c r="E24" t="s">
-        <v>177</v>
-      </c>
       <c r="F24" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -2010,12 +2013,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>96</v>
       </c>
@@ -2026,20 +2029,20 @@
         <v>98</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2047,12 +2050,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>126</v>
       </c>
@@ -2060,137 +2063,137 @@
         <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>84</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>126</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E37" t="s">
+        <v>178</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" t="s">
         <v>179</v>
       </c>
-      <c r="F37" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C38" t="s">
-        <v>176</v>
-      </c>
-      <c r="E38" t="s">
-        <v>180</v>
-      </c>
       <c r="F38" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>96</v>
       </c>
       <c r="E44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F44" t="s">
         <v>98</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>126</v>
       </c>
@@ -2198,124 +2201,124 @@
         <v>91</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>84</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H51" s="25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>126</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E52" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="H52" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" t="s">
         <v>182</v>
       </c>
-      <c r="F52" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C53" t="s">
-        <v>176</v>
-      </c>
-      <c r="E53" t="s">
-        <v>183</v>
-      </c>
       <c r="F53" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>96</v>
       </c>
       <c r="E59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F59" t="s">
         <v>98</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -2323,12 +2326,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>126</v>
       </c>
@@ -2342,10 +2345,10 @@
         <v>100</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>94</v>
       </c>
@@ -2353,9 +2356,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E66" t="s">
         <v>101</v>
@@ -2364,25 +2367,25 @@
         <v>102</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>126</v>
       </c>
@@ -2396,10 +2399,10 @@
         <v>122</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>94</v>
       </c>
@@ -2407,9 +2410,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E72" t="s">
         <v>105</v>
@@ -2418,38 +2421,38 @@
         <v>106</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>94</v>
       </c>
       <c r="B76" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>126</v>
       </c>
@@ -2463,10 +2466,10 @@
         <v>109</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -2474,9 +2477,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E80" t="s">
         <v>110</v>
@@ -2485,10 +2488,10 @@
         <v>111</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="19"/>
       <c r="C81" s="19" t="s">
@@ -2498,22 +2501,22 @@
         <v>91</v>
       </c>
       <c r="E81" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="F81" s="19" t="s">
         <v>253</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>254</v>
       </c>
       <c r="G81" s="19"/>
       <c r="H81" s="14" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>94</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C82" s="19"/>
       <c r="D82" s="19"/>
@@ -2522,7 +2525,7 @@
       <c r="G82" s="19"/>
       <c r="H82" s="19"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>80</v>
       </c>
@@ -2533,25 +2536,25 @@
         <v>113</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -2570,14 +2573,14 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.75" customWidth="1"/>
-    <col min="2" max="2" width="71.08203125" customWidth="1"/>
+    <col min="2" max="2" width="71.125" customWidth="1"/>
     <col min="7" max="7" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>145</v>
       </c>
@@ -2585,21 +2588,21 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2609,18 +2612,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.58203125" customWidth="1"/>
+    <col min="2" max="2" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2631,7 +2634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -2663,26 +2666,34 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2698,17 +2709,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.58203125" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="42.625" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -2722,10 +2733,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2739,10 +2750,10 @@
         <v>77</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -2756,10 +2767,10 @@
         <v>78</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -2773,10 +2784,10 @@
         <v>136</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2790,10 +2801,10 @@
         <v>93</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2804,13 +2815,13 @@
         <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>103</v>
       </c>
@@ -2821,13 +2832,13 @@
         <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -2838,13 +2849,13 @@
         <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -2858,10 +2869,10 @@
         <v>136</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -2875,10 +2886,10 @@
         <v>93</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -2895,253 +2906,253 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
+        <v>192</v>
+      </c>
+      <c r="D19" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="C27" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B19" t="s">
-        <v>187</v>
-      </c>
-      <c r="C19" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" t="s">
-        <v>213</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="B28" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" t="s">
+        <v>220</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B20" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" t="s">
-        <v>214</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
+      <c r="B29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B21" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" t="s">
-        <v>215</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="B30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B22" t="s">
-        <v>190</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D22" t="s">
-        <v>216</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+      <c r="B31" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" t="s">
+        <v>219</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D23" t="s">
-        <v>217</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B24" t="s">
-        <v>192</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D24" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B28" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" t="s">
-        <v>206</v>
-      </c>
-      <c r="D28" t="s">
-        <v>221</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B29" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D29" t="s">
-        <v>222</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" t="s">
         <v>223</v>
       </c>
-      <c r="E30" s="20" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B31" t="s">
-        <v>204</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D31" t="s">
-        <v>220</v>
-      </c>
-      <c r="E31" s="20" t="s">
+      <c r="E32" s="20" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32" t="s">
-        <v>205</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D32" t="s">
-        <v>224</v>
-      </c>
-      <c r="E32" s="20" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="E34" s="23" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="C34" s="23" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="B35" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="C35" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="E35" s="23" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>279</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3158,20 +3169,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.875" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="47.08203125" customWidth="1"/>
-    <col min="8" max="8" width="38.83203125" customWidth="1"/>
+    <col min="7" max="7" width="47.125" customWidth="1"/>
+    <col min="8" max="8" width="38.875" customWidth="1"/>
     <col min="9" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -3197,7 +3208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3242,20 +3253,20 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.08203125" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="29.08203125" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="23" customWidth="1"/>
+    <col min="6" max="6" width="29.125" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="23.58203125" customWidth="1"/>
+    <col min="8" max="8" width="23.625" customWidth="1"/>
     <col min="9" max="1026" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3269,7 +3280,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F1" t="s">
         <v>35</v>
@@ -3278,10 +3289,10 @@
         <v>36</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3289,7 +3300,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3297,7 +3308,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3308,10 +3319,10 @@
         <v>71</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>40</v>
       </c>
@@ -3319,7 +3330,7 @@
         <v>20190826</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -3327,7 +3338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3338,10 +3349,10 @@
         <v>44</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -3352,21 +3363,21 @@
         <v>47</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F9" t="s">
         <v>288</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>289</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>290</v>
-      </c>
-      <c r="H9" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3388,16 +3399,16 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="22.58203125" customWidth="1"/>
-    <col min="4" max="4" width="20.08203125" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -3414,7 +3425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>51</v>
       </c>
@@ -3431,7 +3442,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>51</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>51</v>
       </c>
@@ -3465,7 +3476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -3482,7 +3493,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -3499,7 +3510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -3516,7 +3527,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>

</xml_diff>